<commit_message>
2019 and 2020 - werid stuff with 2020
</commit_message>
<xml_diff>
--- a/2018/Cameras_2018_work.xlsx
+++ b/2018/Cameras_2018_work.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84E9AF32-E765-B641-A16E-5F3AA76C9153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29517496-4BE2-5748-AA12-B69612F88E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15500" xr2:uid="{E0E44275-B49D-9E44-881B-21CCB70C8C48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -719,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7871D4D-7FB9-D740-A23B-E16ACB46A8CB}">
-  <dimension ref="A1:S79"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3728,12 +3728,6 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F79" s="5">
-        <f>SUM(F2:F78)</f>
-        <v>2759</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>